<commit_message>
Excel con template y acomodo de funciones
</commit_message>
<xml_diff>
--- a/Library_benchmark/Resource/DummyReport.xlsx
+++ b/Library_benchmark/Resource/DummyReport.xlsx
@@ -63,7 +63,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor rgb="FF00008B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -98,22 +98,27 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00008B"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -450,15 +455,15 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="3"/>
-    <col min="5" max="8" width="9.140625" style="4"/>
+    <col min="1" max="4" width="9.140625" style="2"/>
+    <col min="5" max="8" width="9.140625" style="3"/>
     <col min="9" max="26" width="9.140625" style="1"/>
-    <col min="27" max="16384" width="9.140625" style="5"/>
+    <col min="27" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="51" customHeight="1">
@@ -469,12 +474,12 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:26" s="1" customFormat="1" ht="51" customHeight="1">
       <c r="I2" s="6"/>
@@ -482,41 +487,41 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:26" s="1" customFormat="1"/>
     <row r="4" spans="1:26" s="1" customFormat="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Cambio para version final
</commit_message>
<xml_diff>
--- a/Library_benchmark/Resource/DummyReport.xlsx
+++ b/Library_benchmark/Resource/DummyReport.xlsx
@@ -95,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -104,10 +104,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,25 +457,29 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="2"/>
-    <col min="5" max="8" width="9.140625" style="3"/>
-    <col min="9" max="26" width="9.140625" style="1"/>
+    <col min="1" max="6" width="9.140625" style="2"/>
+    <col min="7" max="12" width="9.140625" style="3"/>
+    <col min="13" max="26" width="9.140625" style="1"/>
     <col min="27" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="51" customHeight="1">
-      <c r="I1" s="6" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -482,11 +488,15 @@
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:26" s="1" customFormat="1" ht="51" customHeight="1">
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -494,34 +504,43 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:26" s="1" customFormat="1"/>
+    <row r="3" spans="1:26" s="1" customFormat="1">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
     <row r="4" spans="1:26" s="1" customFormat="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>